<commit_message>
conserto na figura 5
</commit_message>
<xml_diff>
--- a/TFET2/Calc_Ron_EL.xlsx
+++ b/TFET2/Calc_Ron_EL.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ionioff" sheetId="2" r:id="rId2"/>
+    <sheet name="FOMs" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="112">
   <si>
     <t>Capacitâncias</t>
   </si>
@@ -214,17 +216,173 @@
   </si>
   <si>
     <t>Ion (0,5V)</t>
+  </si>
+  <si>
+    <t>VDD (V)</t>
+  </si>
+  <si>
+    <t>I_d</t>
+  </si>
+  <si>
+    <t>IOFF I_s</t>
+  </si>
+  <si>
+    <t>Ioff (0V)</t>
+  </si>
+  <si>
+    <t>Ioff (+1V)</t>
+  </si>
+  <si>
+    <t>Ion</t>
+  </si>
+  <si>
+    <t>VGS</t>
+  </si>
+  <si>
+    <t>0.5V</t>
+  </si>
+  <si>
+    <t>0V</t>
+  </si>
+  <si>
+    <t>1V</t>
+  </si>
+  <si>
+    <t>VPG</t>
+  </si>
+  <si>
+    <t>menos 1V</t>
+  </si>
+  <si>
+    <t>Ron (0V)</t>
+  </si>
+  <si>
+    <t>Ron (1V)</t>
+  </si>
+  <si>
+    <t>(i)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ioff=ID(VGS=0V) para </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VPG=-1V, (LP), VBG=0V </t>
+  </si>
+  <si>
+    <t>e alpha=0.5 (NC)</t>
+  </si>
+  <si>
+    <t>(ii)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ion=ID(VGS=0.5V) para </t>
+  </si>
+  <si>
+    <t>(Iiii)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VPG=-1V, (LP), VBG=1V (FBB) </t>
+  </si>
+  <si>
+    <t>(iv)</t>
+  </si>
+  <si>
+    <t>(v)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VPG=+1V, (HP), VBG=0V </t>
+  </si>
+  <si>
+    <t>(vi)</t>
+  </si>
+  <si>
+    <t>(vii)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VPG=+1V, (HP), VBG=1V (FBB) </t>
+  </si>
+  <si>
+    <t>(viii)</t>
+  </si>
+  <si>
+    <t>(iii)</t>
+  </si>
+  <si>
+    <t>Ion/Ioff</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>VPG=-+1V (HP),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBG = 0V </t>
+  </si>
+  <si>
+    <t>e VGS = O valor que dar 0.5V</t>
+  </si>
+  <si>
+    <t>alpha = 0.5 (NC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBG = 1V (FBB) </t>
+  </si>
+  <si>
+    <t>VPG=--1V (LP),</t>
+  </si>
+  <si>
+    <t>Ron incluindo o efeito NC</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>ID(VGS=0.5V)</t>
+  </si>
+  <si>
+    <t>α=0.4</t>
+  </si>
+  <si>
+    <t>α=0.5</t>
+  </si>
+  <si>
+    <t>subthreshold slope</t>
+  </si>
+  <si>
+    <t>Fig 5</t>
+  </si>
+  <si>
+    <t>α=0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">α=0 </t>
+  </si>
+  <si>
+    <t>(mmFET)</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -350,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -371,6 +529,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,7 +546,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:C47"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,11 +853,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
       <c r="H1" t="s">
         <v>20</v>
       </c>
@@ -879,10 +1047,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="3">
         <v>60</v>
       </c>
@@ -1224,7 +1392,7 @@
         <v>0.5</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="11"/>
+        <f>C23/B23</f>
         <v>60479.969034255861</v>
       </c>
       <c r="E23" s="16">
@@ -1582,7 +1750,7 @@
       <c r="B45" s="17">
         <v>0.4</v>
       </c>
-      <c r="C45" s="22">
+      <c r="C45" s="18">
         <v>1.04391307E-8</v>
       </c>
     </row>
@@ -1593,7 +1761,7 @@
       <c r="B46" s="17">
         <v>0.5</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="18">
         <v>1.2492864740000001E-8</v>
       </c>
     </row>
@@ -1604,7 +1772,7 @@
       <c r="B47" s="17">
         <v>0.6</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="18">
         <v>1.4817796249999999E-8</v>
       </c>
     </row>
@@ -1620,31 +1788,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="21"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -1682,7 +1850,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1720,7 +1888,7 @@
         <v>9.532803508E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1758,7 +1926,7 @@
         <v>2.840828682E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>28</v>
       </c>
@@ -1796,24 +1964,24 @@
         <v>335.56418126871102</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="19" t="s">
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="21"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1851,7 +2019,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1889,7 +2057,7 @@
         <v>1.190099874E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -1926,8 +2094,11 @@
       <c r="L10" s="9">
         <v>5.3410755290000004E-13</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>28</v>
       </c>
@@ -1965,7 +2136,12 @@
         <v>222820.26673058901</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1976,7 +2152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1987,7 +2163,7 @@
         <v>1.165620482E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
@@ -2005,4 +2181,795 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.0500000000000001E-16</v>
+      </c>
+      <c r="C2" s="4">
+        <v>4.7099999999999997E-17</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>4.7549926480000001E-8</v>
+      </c>
+      <c r="F2">
+        <v>2.164582017E-7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>30383.319498295299</v>
+      </c>
+      <c r="I2" s="1">
+        <v>22303.332866771001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.0500000000000001E-16</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4.7099999999999997E-17</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>2.1012408190000001E-14</v>
+      </c>
+      <c r="F3">
+        <v>3.0268314979999998E-15</v>
+      </c>
+      <c r="H3" s="1">
+        <v>66069739.4494946</v>
+      </c>
+      <c r="I3" s="1">
+        <v>62785356.084649801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="14">
+        <v>8.2671553319999996E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1.0246011119999999E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1.11120186E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="14">
+        <v>1.231559485E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="14">
+        <v>6.9788227810000002E-9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="14">
+        <v>8.644001533E-9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="14">
+        <v>1.165678882E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="14">
+        <v>2.6937595640000002E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="7.54296875" customWidth="1"/>
+    <col min="10" max="10" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="25">
+        <v>0</v>
+      </c>
+      <c r="C2" s="25">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="25">
+        <v>0</v>
+      </c>
+      <c r="E2" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="25">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>81</v>
+      </c>
+      <c r="R3" t="s">
+        <v>82</v>
+      </c>
+      <c r="S3" t="s">
+        <v>79</v>
+      </c>
+      <c r="T3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="25">
+        <v>0</v>
+      </c>
+      <c r="C4" s="25">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>83</v>
+      </c>
+      <c r="R4" t="s">
+        <v>78</v>
+      </c>
+      <c r="S4" t="s">
+        <v>84</v>
+      </c>
+      <c r="T4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="25">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" t="s">
+        <v>84</v>
+      </c>
+      <c r="T5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="25">
+        <v>0</v>
+      </c>
+      <c r="C7" s="25">
+        <v>1</v>
+      </c>
+      <c r="D7" s="25">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="25">
+        <v>1</v>
+      </c>
+      <c r="D8" s="25">
+        <v>0</v>
+      </c>
+      <c r="E8" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>86</v>
+      </c>
+      <c r="R8" t="s">
+        <v>78</v>
+      </c>
+      <c r="S8" t="s">
+        <v>87</v>
+      </c>
+      <c r="T8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="25">
+        <v>0</v>
+      </c>
+      <c r="C9" s="25">
+        <v>1</v>
+      </c>
+      <c r="D9" s="25">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>88</v>
+      </c>
+      <c r="R9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S9" t="s">
+        <v>87</v>
+      </c>
+      <c r="T9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="25">
+        <v>1</v>
+      </c>
+      <c r="D10" s="25">
+        <v>1</v>
+      </c>
+      <c r="E10" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>89</v>
+      </c>
+      <c r="R10" t="s">
+        <v>78</v>
+      </c>
+      <c r="S10" t="s">
+        <v>90</v>
+      </c>
+      <c r="T10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Q11" t="s">
+        <v>91</v>
+      </c>
+      <c r="R11" t="s">
+        <v>82</v>
+      </c>
+      <c r="S11" t="s">
+        <v>90</v>
+      </c>
+      <c r="T11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="J13" t="s">
+        <v>107</v>
+      </c>
+      <c r="L13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="25">
+        <v>-1</v>
+      </c>
+      <c r="C15" s="25">
+        <v>0</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="J15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" s="17">
+        <v>95</v>
+      </c>
+      <c r="M15" s="17">
+        <v>77</v>
+      </c>
+      <c r="N15" s="17">
+        <v>67</v>
+      </c>
+      <c r="O15" s="17">
+        <v>54</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R15" t="s">
+        <v>95</v>
+      </c>
+      <c r="S15" t="s">
+        <v>96</v>
+      </c>
+      <c r="T15" t="s">
+        <v>97</v>
+      </c>
+      <c r="V15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="25">
+        <v>-1</v>
+      </c>
+      <c r="C16" s="25">
+        <v>0</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="J16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K16" t="s">
+        <v>103</v>
+      </c>
+      <c r="L16" s="27">
+        <v>8.2671553319999996E-6</v>
+      </c>
+      <c r="M16" s="27">
+        <v>1.0154307589999999E-5</v>
+      </c>
+      <c r="N16" s="27">
+        <v>1.1033270979999999E-5</v>
+      </c>
+      <c r="O16" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>81</v>
+      </c>
+      <c r="R16" t="s">
+        <v>95</v>
+      </c>
+      <c r="S16" t="s">
+        <v>99</v>
+      </c>
+      <c r="T16" t="s">
+        <v>97</v>
+      </c>
+      <c r="U16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="25">
+        <v>-1</v>
+      </c>
+      <c r="C17" s="25">
+        <v>1</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="25">
+        <v>-1</v>
+      </c>
+      <c r="C18" s="25">
+        <v>1</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="Q18" t="s">
+        <v>92</v>
+      </c>
+      <c r="R18" t="s">
+        <v>100</v>
+      </c>
+      <c r="S18" t="s">
+        <v>96</v>
+      </c>
+      <c r="T18" t="s">
+        <v>97</v>
+      </c>
+      <c r="V18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Q19" t="s">
+        <v>85</v>
+      </c>
+      <c r="R19" t="s">
+        <v>100</v>
+      </c>
+      <c r="S19" t="s">
+        <v>99</v>
+      </c>
+      <c r="T19" t="s">
+        <v>97</v>
+      </c>
+      <c r="U19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>